<commit_message>
Updated to have correct Length M8 Bolts and Nuts
Added Standard M8 nuts and 65mm Partially threaded Bolts
</commit_message>
<xml_diff>
--- a/JoesDrive_V2 BOM.xlsx
+++ b/JoesDrive_V2 BOM.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d42c44b83a4bbc46/Documents/3D Printing/Robotics and Androids/BB8/James BB8 Project v5 JDV2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jvanduse\Downloads\James BB8 Project v5 JDV2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="368" documentId="11_BE9DE99AA47B2B8EE8586A6619BF5A40F3477B36" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{594AB6A1-9D2B-4E6F-B2A4-94A8A0C8299C}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA320CB1-C9EC-45E2-A8E5-8FD23FC1B948}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29970" yWindow="1170" windowWidth="21600" windowHeight="11175" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Sheet 1'!$A$2:$Z$99</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Sheet 1'!$A$2:$Z$101</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="193">
   <si>
     <t>BOM</t>
   </si>
@@ -986,6 +986,18 @@
   <si>
     <t>Or you can Purchase Adafruit Feather Proto M0</t>
   </si>
+  <si>
+    <t>https://www.mcmaster.com/90592A022</t>
+  </si>
+  <si>
+    <t>M8 Nut (100pk)</t>
+  </si>
+  <si>
+    <t>M8 x 65mm (10pk)</t>
+  </si>
+  <si>
+    <t>https://www.mcmaster.com/90854A415</t>
+  </si>
 </sst>
 </file>
 
@@ -1402,7 +1414,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="88">
+  <cellXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1592,44 +1604,8 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="17" fillId="0" borderId="12" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1662,6 +1638,45 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="7" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="17" fillId="0" borderId="12" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="17" fillId="0" borderId="12" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -1883,13 +1898,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z976"/>
+  <dimension ref="A1:Z978"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B27" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B69" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="F36" sqref="F36:G36"/>
+      <selection pane="bottomRight" activeCell="A78" sqref="A78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="19.5" customHeight="1"/>
@@ -1907,17 +1922,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="19.5" customHeight="1">
-      <c r="A1" s="63" t="s">
+      <c r="A1" s="78" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="64"/>
-      <c r="C1" s="64"/>
-      <c r="D1" s="64"/>
-      <c r="E1" s="64"/>
-      <c r="F1" s="64"/>
-      <c r="G1" s="64"/>
-      <c r="H1" s="64"/>
-      <c r="I1" s="64"/>
+      <c r="B1" s="79"/>
+      <c r="C1" s="79"/>
+      <c r="D1" s="79"/>
+      <c r="E1" s="79"/>
+      <c r="F1" s="79"/>
+      <c r="G1" s="79"/>
+      <c r="H1" s="79"/>
+      <c r="I1" s="79"/>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
@@ -1960,8 +1975,8 @@
       </c>
       <c r="H2" s="5"/>
       <c r="I2" s="6">
-        <f>SUM(E108,E99,E95,E76,E46,E40,E14)</f>
-        <v>1224.6500000000001</v>
+        <f>SUM(E110,E101,E97,E78,E46,E40,E14)</f>
+        <v>1241.9900000000002</v>
       </c>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
@@ -2012,31 +2027,31 @@
       <c r="Z3" s="1"/>
     </row>
     <row r="4" spans="1:26" ht="19.5" customHeight="1">
-      <c r="A4" s="76" t="s">
+      <c r="A4" s="64" t="s">
         <v>152</v>
       </c>
-      <c r="B4" s="77">
+      <c r="B4" s="65">
         <v>1</v>
       </c>
-      <c r="C4" s="78">
+      <c r="C4" s="66">
         <v>1</v>
       </c>
-      <c r="D4" s="79">
+      <c r="D4" s="67">
         <v>24.95</v>
       </c>
-      <c r="E4" s="79">
+      <c r="E4" s="67">
         <f t="shared" ref="E4:E13" si="0">D4*C4</f>
         <v>24.95</v>
       </c>
-      <c r="F4" s="80" t="s">
+      <c r="F4" s="68" t="s">
         <v>179</v>
       </c>
-      <c r="G4" s="78"/>
-      <c r="H4" s="81" t="str">
+      <c r="G4" s="66"/>
+      <c r="H4" s="69" t="str">
         <f t="shared" ref="H4:H9" si="1">IF(F4&gt;0,LEFT(F4,20),"ZZZ")</f>
         <v>https://www.adafruit</v>
       </c>
-      <c r="I4" s="78"/>
+      <c r="I4" s="66"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
@@ -2056,28 +2071,28 @@
       <c r="Z4" s="1"/>
     </row>
     <row r="5" spans="1:26" s="61" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A5" s="76" t="s">
+      <c r="A5" s="64" t="s">
         <v>188</v>
       </c>
-      <c r="B5" s="82">
+      <c r="B5" s="70">
         <v>1</v>
       </c>
-      <c r="C5" s="83">
+      <c r="C5" s="71">
         <v>1</v>
       </c>
-      <c r="D5" s="84">
+      <c r="D5" s="72">
         <v>19.95</v>
       </c>
-      <c r="E5" s="79">
+      <c r="E5" s="67">
         <f t="shared" si="0"/>
         <v>19.95</v>
       </c>
-      <c r="F5" s="85" t="s">
+      <c r="F5" s="73" t="s">
         <v>185</v>
       </c>
-      <c r="G5" s="83"/>
-      <c r="H5" s="86"/>
-      <c r="I5" s="83"/>
+      <c r="G5" s="71"/>
+      <c r="H5" s="74"/>
+      <c r="I5" s="71"/>
     </row>
     <row r="6" spans="1:26" ht="19.5" customHeight="1">
       <c r="A6" s="13" t="s">
@@ -3089,10 +3104,10 @@
         <f t="shared" ref="E32:E34" si="4">D32*C32</f>
         <v>48.34</v>
       </c>
-      <c r="F32" s="71" t="s">
+      <c r="F32" s="84" t="s">
         <v>35</v>
       </c>
-      <c r="G32" s="72"/>
+      <c r="G32" s="85"/>
       <c r="H32" s="40"/>
       <c r="I32" s="15"/>
       <c r="J32" s="1"/>
@@ -3130,10 +3145,10 @@
         <f>D33*C33</f>
         <v>5.99</v>
       </c>
-      <c r="F33" s="71" t="s">
+      <c r="F33" s="84" t="s">
         <v>37</v>
       </c>
-      <c r="G33" s="72"/>
+      <c r="G33" s="85"/>
       <c r="H33" s="40"/>
       <c r="I33" s="15"/>
       <c r="J33" s="1"/>
@@ -3171,10 +3186,10 @@
         <f t="shared" si="4"/>
         <v>11.99</v>
       </c>
-      <c r="F34" s="71" t="s">
+      <c r="F34" s="84" t="s">
         <v>39</v>
       </c>
-      <c r="G34" s="72"/>
+      <c r="G34" s="85"/>
       <c r="H34" s="40"/>
       <c r="I34" s="15"/>
       <c r="J34" s="1"/>
@@ -3212,10 +3227,10 @@
         <f t="shared" ref="E35" si="5">D35*C35</f>
         <v>5.6</v>
       </c>
-      <c r="F35" s="71" t="s">
+      <c r="F35" s="84" t="s">
         <v>41</v>
       </c>
-      <c r="G35" s="72"/>
+      <c r="G35" s="85"/>
       <c r="H35" s="40"/>
       <c r="I35" s="15"/>
       <c r="J35" s="1"/>
@@ -3253,10 +3268,10 @@
         <f t="shared" ref="E36:E38" si="6">D36*C36</f>
         <v>8.99</v>
       </c>
-      <c r="F36" s="87" t="s">
+      <c r="F36" s="88" t="s">
         <v>153</v>
       </c>
-      <c r="G36" s="72"/>
+      <c r="G36" s="85"/>
       <c r="H36" s="40"/>
       <c r="I36" s="33"/>
     </row>
@@ -3277,10 +3292,10 @@
         <f t="shared" si="6"/>
         <v>7.99</v>
       </c>
-      <c r="F37" s="87" t="s">
+      <c r="F37" s="88" t="s">
         <v>156</v>
       </c>
-      <c r="G37" s="72"/>
+      <c r="G37" s="85"/>
       <c r="H37" s="40"/>
       <c r="I37" s="33"/>
     </row>
@@ -3301,10 +3316,10 @@
         <f t="shared" si="6"/>
         <v>7.99</v>
       </c>
-      <c r="F38" s="71" t="s">
+      <c r="F38" s="84" t="s">
         <v>157</v>
       </c>
-      <c r="G38" s="72"/>
+      <c r="G38" s="85"/>
       <c r="H38" s="40"/>
       <c r="I38" s="33"/>
     </row>
@@ -3324,10 +3339,10 @@
       <c r="E39" s="16">
         <v>5</v>
       </c>
-      <c r="F39" s="73" t="s">
+      <c r="F39" s="86" t="s">
         <v>141</v>
       </c>
-      <c r="G39" s="74"/>
+      <c r="G39" s="87"/>
       <c r="H39" s="40"/>
       <c r="I39" s="15"/>
       <c r="J39" s="1"/>
@@ -3452,10 +3467,10 @@
       <c r="E43" s="16">
         <v>5</v>
       </c>
-      <c r="F43" s="65" t="s">
+      <c r="F43" s="80" t="s">
         <v>139</v>
       </c>
-      <c r="G43" s="66"/>
+      <c r="G43" s="81"/>
       <c r="H43" s="18"/>
       <c r="I43" s="33"/>
     </row>
@@ -3506,10 +3521,10 @@
         <f>D45*C45</f>
         <v>58</v>
       </c>
-      <c r="F45" s="67" t="s">
+      <c r="F45" s="77" t="s">
         <v>47</v>
       </c>
-      <c r="G45" s="68"/>
+      <c r="G45" s="76"/>
       <c r="H45" s="40" t="str">
         <f>IF(F45&gt;0,LEFT(F45,20),"ZZZ")</f>
         <v>https://www.dfrobot.</v>
@@ -3542,8 +3557,8 @@
         <f>SUM(E45)</f>
         <v>58</v>
       </c>
-      <c r="F46" s="69"/>
-      <c r="G46" s="70"/>
+      <c r="F46" s="82"/>
+      <c r="G46" s="83"/>
       <c r="H46" s="40"/>
       <c r="I46" s="15"/>
       <c r="J46" s="1"/>
@@ -3611,12 +3626,12 @@
         <f t="shared" ref="E48:E49" si="7">D48*C48</f>
         <v>2.4</v>
       </c>
-      <c r="F48" s="67" t="s">
+      <c r="F48" s="77" t="s">
         <v>50</v>
       </c>
-      <c r="G48" s="68"/>
+      <c r="G48" s="76"/>
       <c r="H48" s="18" t="str">
-        <f t="shared" ref="H48:H75" si="8">IF(F48&gt;0,LEFT(F48,20),"ZZZ")</f>
+        <f t="shared" ref="H48:H76" si="8">IF(F48&gt;0,LEFT(F48,20),"ZZZ")</f>
         <v>https://www.mcmaster</v>
       </c>
       <c r="I48" s="15"/>
@@ -3655,10 +3670,10 @@
         <f t="shared" si="7"/>
         <v>2.94</v>
       </c>
-      <c r="F49" s="67" t="s">
+      <c r="F49" s="77" t="s">
         <v>52</v>
       </c>
-      <c r="G49" s="68"/>
+      <c r="G49" s="76"/>
       <c r="H49" s="18" t="str">
         <f t="shared" si="8"/>
         <v>https://www.mcmaster</v>
@@ -3698,10 +3713,10 @@
       <c r="E50" s="36">
         <v>2.19</v>
       </c>
-      <c r="F50" s="67" t="s">
+      <c r="F50" s="77" t="s">
         <v>54</v>
       </c>
-      <c r="G50" s="68"/>
+      <c r="G50" s="76"/>
       <c r="H50" s="18" t="str">
         <f t="shared" si="8"/>
         <v>https://www.mcmaster</v>
@@ -3739,13 +3754,13 @@
         <v>1.2</v>
       </c>
       <c r="E51" s="16">
-        <f t="shared" ref="E51:E75" si="9">D51*C51</f>
+        <f t="shared" ref="E51:E77" si="9">D51*C51</f>
         <v>1.2</v>
       </c>
-      <c r="F51" s="67" t="s">
+      <c r="F51" s="77" t="s">
         <v>56</v>
       </c>
-      <c r="G51" s="68"/>
+      <c r="G51" s="76"/>
       <c r="H51" s="18" t="str">
         <f t="shared" si="8"/>
         <v>https://www.mcmaster</v>
@@ -3786,10 +3801,10 @@
         <f t="shared" si="9"/>
         <v>3.77</v>
       </c>
-      <c r="F52" s="67" t="s">
+      <c r="F52" s="77" t="s">
         <v>58</v>
       </c>
-      <c r="G52" s="68"/>
+      <c r="G52" s="76"/>
       <c r="H52" s="18" t="str">
         <f t="shared" si="8"/>
         <v>https://www.mcmaster</v>
@@ -4737,69 +4752,49 @@
       <c r="Y73" s="1"/>
       <c r="Z73" s="1"/>
     </row>
-    <row r="74" spans="1:26" ht="19.5" customHeight="1">
+    <row r="74" spans="1:26" s="63" customFormat="1" ht="19.5" customHeight="1">
       <c r="A74" s="34" t="s">
+        <v>190</v>
+      </c>
+      <c r="B74" s="35">
+        <v>4</v>
+      </c>
+      <c r="C74" s="33">
+        <v>1</v>
+      </c>
+      <c r="D74" s="36">
+        <v>6.14</v>
+      </c>
+      <c r="E74" s="36">
+        <f t="shared" si="9"/>
+        <v>6.14</v>
+      </c>
+      <c r="F74" s="17" t="s">
+        <v>189</v>
+      </c>
+      <c r="G74" s="33"/>
+      <c r="H74" s="18"/>
+      <c r="I74" s="33"/>
+    </row>
+    <row r="75" spans="1:26" ht="19.5" customHeight="1">
+      <c r="A75" s="34" t="s">
         <v>101</v>
       </c>
-      <c r="B74" s="14">
+      <c r="B75" s="14">
         <v>1</v>
       </c>
-      <c r="C74" s="15">
+      <c r="C75" s="15">
         <v>1</v>
       </c>
-      <c r="D74" s="16">
+      <c r="D75" s="16">
         <v>9.14</v>
       </c>
-      <c r="E74" s="16">
+      <c r="E75" s="16">
         <f t="shared" si="9"/>
         <v>9.14</v>
       </c>
-      <c r="F74" s="17" t="s">
+      <c r="F75" s="17" t="s">
         <v>102</v>
-      </c>
-      <c r="G74" s="15"/>
-      <c r="H74" s="18" t="str">
-        <f t="shared" si="8"/>
-        <v>https://www.mcmaster</v>
-      </c>
-      <c r="I74" s="15"/>
-      <c r="J74" s="1"/>
-      <c r="K74" s="1"/>
-      <c r="L74" s="1"/>
-      <c r="M74" s="1"/>
-      <c r="N74" s="1"/>
-      <c r="O74" s="1"/>
-      <c r="P74" s="1"/>
-      <c r="Q74" s="1"/>
-      <c r="R74" s="1"/>
-      <c r="S74" s="1"/>
-      <c r="T74" s="1"/>
-      <c r="U74" s="1"/>
-      <c r="V74" s="1"/>
-      <c r="W74" s="1"/>
-      <c r="X74" s="1"/>
-      <c r="Y74" s="1"/>
-      <c r="Z74" s="1"/>
-    </row>
-    <row r="75" spans="1:26" ht="19.5" customHeight="1">
-      <c r="A75" s="34" t="s">
-        <v>103</v>
-      </c>
-      <c r="B75" s="14">
-        <v>1</v>
-      </c>
-      <c r="C75" s="15">
-        <v>1</v>
-      </c>
-      <c r="D75" s="16">
-        <v>8.91</v>
-      </c>
-      <c r="E75" s="16">
-        <f t="shared" si="9"/>
-        <v>8.91</v>
-      </c>
-      <c r="F75" s="17" t="s">
-        <v>104</v>
       </c>
       <c r="G75" s="15"/>
       <c r="H75" s="18" t="str">
@@ -4826,17 +4821,30 @@
       <c r="Z75" s="1"/>
     </row>
     <row r="76" spans="1:26" ht="19.5" customHeight="1">
-      <c r="A76" s="38"/>
-      <c r="B76" s="35"/>
-      <c r="C76" s="33"/>
-      <c r="D76" s="36"/>
+      <c r="A76" s="34" t="s">
+        <v>103</v>
+      </c>
+      <c r="B76" s="14">
+        <v>1</v>
+      </c>
+      <c r="C76" s="15">
+        <v>1</v>
+      </c>
+      <c r="D76" s="16">
+        <v>8.91</v>
+      </c>
       <c r="E76" s="16">
-        <f>SUM(E48:E75)</f>
-        <v>156.13999999999996</v>
-      </c>
-      <c r="F76" s="46"/>
+        <f t="shared" si="9"/>
+        <v>8.91</v>
+      </c>
+      <c r="F76" s="17" t="s">
+        <v>104</v>
+      </c>
       <c r="G76" s="15"/>
-      <c r="H76" s="40"/>
+      <c r="H76" s="18" t="str">
+        <f t="shared" si="8"/>
+        <v>https://www.mcmaster</v>
+      </c>
       <c r="I76" s="15"/>
       <c r="J76" s="1"/>
       <c r="K76" s="1"/>
@@ -4856,61 +4864,42 @@
       <c r="Y76" s="1"/>
       <c r="Z76" s="1"/>
     </row>
-    <row r="77" spans="1:26" ht="19.5" customHeight="1">
-      <c r="A77" s="41" t="s">
-        <v>105</v>
-      </c>
-      <c r="B77" s="28"/>
-      <c r="C77" s="29"/>
-      <c r="D77" s="30"/>
-      <c r="E77" s="30"/>
-      <c r="F77" s="31"/>
-      <c r="G77" s="29"/>
-      <c r="H77" s="32"/>
-      <c r="I77" s="29"/>
-      <c r="J77" s="1"/>
-      <c r="K77" s="1"/>
-      <c r="L77" s="1"/>
-      <c r="M77" s="1"/>
-      <c r="N77" s="1"/>
-      <c r="O77" s="1"/>
-      <c r="P77" s="1"/>
-      <c r="Q77" s="1"/>
-      <c r="R77" s="1"/>
-      <c r="S77" s="1"/>
-      <c r="T77" s="1"/>
-      <c r="U77" s="1"/>
-      <c r="V77" s="1"/>
-      <c r="W77" s="1"/>
-      <c r="X77" s="1"/>
-      <c r="Y77" s="1"/>
-      <c r="Z77" s="1"/>
+    <row r="77" spans="1:26" s="63" customFormat="1" ht="19.5" customHeight="1">
+      <c r="A77" s="34" t="s">
+        <v>191</v>
+      </c>
+      <c r="B77" s="35">
+        <v>2</v>
+      </c>
+      <c r="C77" s="33">
+        <v>1</v>
+      </c>
+      <c r="D77" s="36">
+        <v>11.2</v>
+      </c>
+      <c r="E77" s="36">
+        <f t="shared" si="9"/>
+        <v>11.2</v>
+      </c>
+      <c r="F77" s="17" t="s">
+        <v>192</v>
+      </c>
+      <c r="G77" s="33"/>
+      <c r="H77" s="18"/>
+      <c r="I77" s="33"/>
     </row>
     <row r="78" spans="1:26" ht="19.5" customHeight="1">
-      <c r="A78" s="13" t="s">
-        <v>106</v>
-      </c>
-      <c r="B78" s="14">
-        <v>1</v>
-      </c>
-      <c r="C78" s="15">
-        <v>1</v>
-      </c>
-      <c r="D78" s="16">
-        <v>4.99</v>
-      </c>
+      <c r="A78" s="38"/>
+      <c r="B78" s="35"/>
+      <c r="C78" s="33"/>
+      <c r="D78" s="36"/>
       <c r="E78" s="16">
-        <f t="shared" ref="E78:E93" si="10">D78*C78</f>
-        <v>4.99</v>
-      </c>
-      <c r="F78" s="17" t="s">
-        <v>107</v>
-      </c>
+        <f>SUM(E48:E77)</f>
+        <v>173.47999999999993</v>
+      </c>
+      <c r="F78" s="46"/>
       <c r="G78" s="15"/>
-      <c r="H78" s="18" t="str">
-        <f t="shared" ref="H78:H93" si="11">IF(F78&gt;0,LEFT(F78,20),"ZZZ")</f>
-        <v>https://www.servocit</v>
-      </c>
+      <c r="H78" s="40"/>
       <c r="I78" s="15"/>
       <c r="J78" s="1"/>
       <c r="K78" s="1"/>
@@ -4931,31 +4920,17 @@
       <c r="Z78" s="1"/>
     </row>
     <row r="79" spans="1:26" ht="19.5" customHeight="1">
-      <c r="A79" s="13" t="s">
-        <v>108</v>
-      </c>
-      <c r="B79" s="14">
-        <v>3</v>
-      </c>
-      <c r="C79" s="15">
-        <v>3</v>
-      </c>
-      <c r="D79" s="16">
-        <v>14.99</v>
-      </c>
-      <c r="E79" s="16">
-        <f t="shared" si="10"/>
-        <v>44.97</v>
-      </c>
-      <c r="F79" s="17" t="s">
-        <v>109</v>
-      </c>
-      <c r="G79" s="15"/>
-      <c r="H79" s="18" t="str">
-        <f t="shared" si="11"/>
-        <v>https://www.servocit</v>
-      </c>
-      <c r="I79" s="15"/>
+      <c r="A79" s="41" t="s">
+        <v>105</v>
+      </c>
+      <c r="B79" s="28"/>
+      <c r="C79" s="29"/>
+      <c r="D79" s="30"/>
+      <c r="E79" s="30"/>
+      <c r="F79" s="31"/>
+      <c r="G79" s="29"/>
+      <c r="H79" s="32"/>
+      <c r="I79" s="29"/>
       <c r="J79" s="1"/>
       <c r="K79" s="1"/>
       <c r="L79" s="1"/>
@@ -4976,27 +4951,27 @@
     </row>
     <row r="80" spans="1:26" ht="19.5" customHeight="1">
       <c r="A80" s="13" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="B80" s="14">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="C80" s="15">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="D80" s="16">
-        <v>9.99</v>
+        <v>4.99</v>
       </c>
       <c r="E80" s="16">
-        <f t="shared" si="10"/>
-        <v>79.92</v>
+        <f t="shared" ref="E80:E95" si="10">D80*C80</f>
+        <v>4.99</v>
       </c>
       <c r="F80" s="17" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="G80" s="15"/>
       <c r="H80" s="18" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" ref="H80:H95" si="11">IF(F80&gt;0,LEFT(F80,20),"ZZZ")</f>
         <v>https://www.servocit</v>
       </c>
       <c r="I80" s="15"/>
@@ -5020,23 +4995,23 @@
     </row>
     <row r="81" spans="1:26" ht="19.5" customHeight="1">
       <c r="A81" s="13" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="B81" s="14">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C81" s="15">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D81" s="16">
-        <v>8.69</v>
+        <v>14.99</v>
       </c>
       <c r="E81" s="16">
         <f t="shared" si="10"/>
-        <v>17.38</v>
+        <v>44.97</v>
       </c>
       <c r="F81" s="17" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="G81" s="15"/>
       <c r="H81" s="18" t="str">
@@ -5063,24 +5038,24 @@
       <c r="Z81" s="1"/>
     </row>
     <row r="82" spans="1:26" ht="19.5" customHeight="1">
-      <c r="A82" s="34" t="s">
-        <v>114</v>
+      <c r="A82" s="13" t="s">
+        <v>110</v>
       </c>
       <c r="B82" s="14">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C82" s="15">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="D82" s="16">
-        <v>39.99</v>
+        <v>9.99</v>
       </c>
       <c r="E82" s="16">
         <f t="shared" si="10"/>
-        <v>39.99</v>
+        <v>79.92</v>
       </c>
       <c r="F82" s="17" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="G82" s="15"/>
       <c r="H82" s="18" t="str">
@@ -5107,24 +5082,24 @@
       <c r="Z82" s="1"/>
     </row>
     <row r="83" spans="1:26" ht="19.5" customHeight="1">
-      <c r="A83" s="34" t="s">
-        <v>116</v>
+      <c r="A83" s="13" t="s">
+        <v>112</v>
       </c>
       <c r="B83" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C83" s="15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D83" s="16">
-        <v>39.99</v>
+        <v>8.69</v>
       </c>
       <c r="E83" s="16">
         <f t="shared" si="10"/>
-        <v>39.99</v>
+        <v>17.38</v>
       </c>
       <c r="F83" s="17" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="G83" s="15"/>
       <c r="H83" s="18" t="str">
@@ -5151,8 +5126,8 @@
       <c r="Z83" s="1"/>
     </row>
     <row r="84" spans="1:26" ht="19.5" customHeight="1">
-      <c r="A84" s="13" t="s">
-        <v>118</v>
+      <c r="A84" s="34" t="s">
+        <v>114</v>
       </c>
       <c r="B84" s="14">
         <v>1</v>
@@ -5161,14 +5136,14 @@
         <v>1</v>
       </c>
       <c r="D84" s="16">
-        <v>3.99</v>
+        <v>39.99</v>
       </c>
       <c r="E84" s="16">
         <f t="shared" si="10"/>
-        <v>3.99</v>
+        <v>39.99</v>
       </c>
       <c r="F84" s="17" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="G84" s="15"/>
       <c r="H84" s="18" t="str">
@@ -5195,8 +5170,8 @@
       <c r="Z84" s="1"/>
     </row>
     <row r="85" spans="1:26" ht="19.5" customHeight="1">
-      <c r="A85" s="13" t="s">
-        <v>120</v>
+      <c r="A85" s="34" t="s">
+        <v>116</v>
       </c>
       <c r="B85" s="14">
         <v>1</v>
@@ -5205,14 +5180,14 @@
         <v>1</v>
       </c>
       <c r="D85" s="16">
-        <v>4.09</v>
+        <v>39.99</v>
       </c>
       <c r="E85" s="16">
         <f t="shared" si="10"/>
-        <v>4.09</v>
+        <v>39.99</v>
       </c>
       <c r="F85" s="17" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="G85" s="15"/>
       <c r="H85" s="18" t="str">
@@ -5240,7 +5215,7 @@
     </row>
     <row r="86" spans="1:26" ht="19.5" customHeight="1">
       <c r="A86" s="13" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="B86" s="14">
         <v>1</v>
@@ -5249,14 +5224,14 @@
         <v>1</v>
       </c>
       <c r="D86" s="16">
-        <v>6.99</v>
+        <v>3.99</v>
       </c>
       <c r="E86" s="16">
         <f t="shared" si="10"/>
-        <v>6.99</v>
+        <v>3.99</v>
       </c>
       <c r="F86" s="17" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="G86" s="15"/>
       <c r="H86" s="18" t="str">
@@ -5283,24 +5258,24 @@
       <c r="Z86" s="1"/>
     </row>
     <row r="87" spans="1:26" ht="19.5" customHeight="1">
-      <c r="A87" s="34" t="s">
-        <v>124</v>
+      <c r="A87" s="13" t="s">
+        <v>120</v>
       </c>
       <c r="B87" s="14">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C87" s="15">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D87" s="16">
-        <v>2.79</v>
+        <v>4.09</v>
       </c>
       <c r="E87" s="16">
         <f t="shared" si="10"/>
-        <v>5.58</v>
+        <v>4.09</v>
       </c>
       <c r="F87" s="17" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="G87" s="15"/>
       <c r="H87" s="18" t="str">
@@ -5326,49 +5301,69 @@
       <c r="Y87" s="1"/>
       <c r="Z87" s="1"/>
     </row>
-    <row r="88" spans="1:26" s="58" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A88" s="60" t="s">
-        <v>178</v>
-      </c>
-      <c r="B88" s="35">
-        <v>2</v>
-      </c>
-      <c r="C88" s="33">
+    <row r="88" spans="1:26" ht="19.5" customHeight="1">
+      <c r="A88" s="13" t="s">
+        <v>122</v>
+      </c>
+      <c r="B88" s="14">
         <v>1</v>
       </c>
-      <c r="D88" s="36">
-        <v>16</v>
-      </c>
-      <c r="E88" s="36">
+      <c r="C88" s="15">
+        <v>1</v>
+      </c>
+      <c r="D88" s="16">
+        <v>6.99</v>
+      </c>
+      <c r="E88" s="16">
         <f t="shared" si="10"/>
-        <v>16</v>
-      </c>
-      <c r="F88" s="75" t="s">
-        <v>177</v>
-      </c>
-      <c r="G88" s="68"/>
-      <c r="H88" s="18"/>
-      <c r="I88" s="33"/>
+        <v>6.99</v>
+      </c>
+      <c r="F88" s="17" t="s">
+        <v>123</v>
+      </c>
+      <c r="G88" s="15"/>
+      <c r="H88" s="18" t="str">
+        <f t="shared" si="11"/>
+        <v>https://www.servocit</v>
+      </c>
+      <c r="I88" s="15"/>
+      <c r="J88" s="1"/>
+      <c r="K88" s="1"/>
+      <c r="L88" s="1"/>
+      <c r="M88" s="1"/>
+      <c r="N88" s="1"/>
+      <c r="O88" s="1"/>
+      <c r="P88" s="1"/>
+      <c r="Q88" s="1"/>
+      <c r="R88" s="1"/>
+      <c r="S88" s="1"/>
+      <c r="T88" s="1"/>
+      <c r="U88" s="1"/>
+      <c r="V88" s="1"/>
+      <c r="W88" s="1"/>
+      <c r="X88" s="1"/>
+      <c r="Y88" s="1"/>
+      <c r="Z88" s="1"/>
     </row>
     <row r="89" spans="1:26" ht="19.5" customHeight="1">
       <c r="A89" s="34" t="s">
-        <v>126</v>
-      </c>
-      <c r="B89" s="35">
+        <v>124</v>
+      </c>
+      <c r="B89" s="14">
         <v>4</v>
       </c>
-      <c r="C89" s="33">
-        <v>4</v>
+      <c r="C89" s="15">
+        <v>2</v>
       </c>
       <c r="D89" s="16">
-        <v>6.99</v>
+        <v>2.79</v>
       </c>
       <c r="E89" s="16">
         <f t="shared" si="10"/>
-        <v>27.96</v>
-      </c>
-      <c r="F89" s="37" t="s">
-        <v>127</v>
+        <v>5.58</v>
+      </c>
+      <c r="F89" s="17" t="s">
+        <v>125</v>
       </c>
       <c r="G89" s="15"/>
       <c r="H89" s="18" t="str">
@@ -5394,69 +5389,49 @@
       <c r="Y89" s="1"/>
       <c r="Z89" s="1"/>
     </row>
-    <row r="90" spans="1:26" ht="19.5" customHeight="1">
-      <c r="A90" s="13" t="s">
-        <v>128</v>
-      </c>
-      <c r="B90" s="14">
+    <row r="90" spans="1:26" s="58" customFormat="1" ht="19.5" customHeight="1">
+      <c r="A90" s="60" t="s">
+        <v>178</v>
+      </c>
+      <c r="B90" s="35">
+        <v>2</v>
+      </c>
+      <c r="C90" s="33">
         <v>1</v>
       </c>
-      <c r="C90" s="15">
-        <v>1</v>
-      </c>
-      <c r="D90" s="16">
-        <v>6.39</v>
-      </c>
-      <c r="E90" s="16">
+      <c r="D90" s="36">
+        <v>16</v>
+      </c>
+      <c r="E90" s="36">
         <f t="shared" si="10"/>
-        <v>6.39</v>
-      </c>
-      <c r="F90" s="17" t="s">
-        <v>129</v>
-      </c>
-      <c r="G90" s="15"/>
-      <c r="H90" s="18" t="str">
-        <f t="shared" si="11"/>
-        <v>https://www.servocit</v>
-      </c>
-      <c r="I90" s="15"/>
-      <c r="J90" s="1"/>
-      <c r="K90" s="1"/>
-      <c r="L90" s="1"/>
-      <c r="M90" s="1"/>
-      <c r="N90" s="1"/>
-      <c r="O90" s="1"/>
-      <c r="P90" s="1"/>
-      <c r="Q90" s="1"/>
-      <c r="R90" s="1"/>
-      <c r="S90" s="1"/>
-      <c r="T90" s="1"/>
-      <c r="U90" s="1"/>
-      <c r="V90" s="1"/>
-      <c r="W90" s="1"/>
-      <c r="X90" s="1"/>
-      <c r="Y90" s="1"/>
-      <c r="Z90" s="1"/>
+        <v>16</v>
+      </c>
+      <c r="F90" s="75" t="s">
+        <v>177</v>
+      </c>
+      <c r="G90" s="76"/>
+      <c r="H90" s="18"/>
+      <c r="I90" s="33"/>
     </row>
     <row r="91" spans="1:26" ht="19.5" customHeight="1">
-      <c r="A91" s="13" t="s">
-        <v>130</v>
-      </c>
-      <c r="B91" s="14">
-        <v>2</v>
-      </c>
-      <c r="C91" s="15">
-        <v>2</v>
+      <c r="A91" s="34" t="s">
+        <v>126</v>
+      </c>
+      <c r="B91" s="35">
+        <v>4</v>
+      </c>
+      <c r="C91" s="33">
+        <v>4</v>
       </c>
       <c r="D91" s="16">
         <v>6.99</v>
       </c>
       <c r="E91" s="16">
         <f t="shared" si="10"/>
-        <v>13.98</v>
-      </c>
-      <c r="F91" s="17" t="s">
-        <v>131</v>
+        <v>27.96</v>
+      </c>
+      <c r="F91" s="37" t="s">
+        <v>127</v>
       </c>
       <c r="G91" s="15"/>
       <c r="H91" s="18" t="str">
@@ -5484,7 +5459,7 @@
     </row>
     <row r="92" spans="1:26" ht="19.5" customHeight="1">
       <c r="A92" s="13" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="B92" s="14">
         <v>1</v>
@@ -5493,14 +5468,14 @@
         <v>1</v>
       </c>
       <c r="D92" s="16">
-        <v>5.99</v>
+        <v>6.39</v>
       </c>
       <c r="E92" s="16">
         <f t="shared" si="10"/>
-        <v>5.99</v>
+        <v>6.39</v>
       </c>
       <c r="F92" s="17" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="G92" s="15"/>
       <c r="H92" s="18" t="str">
@@ -5528,23 +5503,23 @@
     </row>
     <row r="93" spans="1:26" ht="19.5" customHeight="1">
       <c r="A93" s="13" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="B93" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C93" s="15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D93" s="16">
-        <v>5.99</v>
+        <v>6.99</v>
       </c>
       <c r="E93" s="16">
         <f t="shared" si="10"/>
-        <v>5.99</v>
+        <v>13.98</v>
       </c>
       <c r="F93" s="17" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="G93" s="15"/>
       <c r="H93" s="18" t="str">
@@ -5570,221 +5545,261 @@
       <c r="Y93" s="1"/>
       <c r="Z93" s="1"/>
     </row>
-    <row r="94" spans="1:26" s="48" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A94" s="34" t="s">
+    <row r="94" spans="1:26" ht="19.5" customHeight="1">
+      <c r="A94" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="B94" s="14">
+        <v>1</v>
+      </c>
+      <c r="C94" s="15">
+        <v>1</v>
+      </c>
+      <c r="D94" s="16">
+        <v>5.99</v>
+      </c>
+      <c r="E94" s="16">
+        <f t="shared" si="10"/>
+        <v>5.99</v>
+      </c>
+      <c r="F94" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="G94" s="15"/>
+      <c r="H94" s="18" t="str">
+        <f t="shared" si="11"/>
+        <v>https://www.servocit</v>
+      </c>
+      <c r="I94" s="15"/>
+      <c r="J94" s="1"/>
+      <c r="K94" s="1"/>
+      <c r="L94" s="1"/>
+      <c r="M94" s="1"/>
+      <c r="N94" s="1"/>
+      <c r="O94" s="1"/>
+      <c r="P94" s="1"/>
+      <c r="Q94" s="1"/>
+      <c r="R94" s="1"/>
+      <c r="S94" s="1"/>
+      <c r="T94" s="1"/>
+      <c r="U94" s="1"/>
+      <c r="V94" s="1"/>
+      <c r="W94" s="1"/>
+      <c r="X94" s="1"/>
+      <c r="Y94" s="1"/>
+      <c r="Z94" s="1"/>
+    </row>
+    <row r="95" spans="1:26" ht="19.5" customHeight="1">
+      <c r="A95" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="B95" s="14">
+        <v>1</v>
+      </c>
+      <c r="C95" s="15">
+        <v>1</v>
+      </c>
+      <c r="D95" s="16">
+        <v>5.99</v>
+      </c>
+      <c r="E95" s="16">
+        <f t="shared" si="10"/>
+        <v>5.99</v>
+      </c>
+      <c r="F95" s="17" t="s">
+        <v>135</v>
+      </c>
+      <c r="G95" s="15"/>
+      <c r="H95" s="18" t="str">
+        <f t="shared" si="11"/>
+        <v>https://www.servocit</v>
+      </c>
+      <c r="I95" s="15"/>
+      <c r="J95" s="1"/>
+      <c r="K95" s="1"/>
+      <c r="L95" s="1"/>
+      <c r="M95" s="1"/>
+      <c r="N95" s="1"/>
+      <c r="O95" s="1"/>
+      <c r="P95" s="1"/>
+      <c r="Q95" s="1"/>
+      <c r="R95" s="1"/>
+      <c r="S95" s="1"/>
+      <c r="T95" s="1"/>
+      <c r="U95" s="1"/>
+      <c r="V95" s="1"/>
+      <c r="W95" s="1"/>
+      <c r="X95" s="1"/>
+      <c r="Y95" s="1"/>
+      <c r="Z95" s="1"/>
+    </row>
+    <row r="96" spans="1:26" s="48" customFormat="1" ht="19.5" customHeight="1">
+      <c r="A96" s="34" t="s">
         <v>136</v>
       </c>
-      <c r="B94" s="35">
+      <c r="B96" s="35">
         <v>1</v>
       </c>
-      <c r="C94" s="33">
+      <c r="C96" s="33">
         <v>1</v>
       </c>
-      <c r="D94" s="36">
+      <c r="D96" s="36">
         <v>25</v>
       </c>
-      <c r="E94" s="36">
+      <c r="E96" s="36">
         <v>25</v>
       </c>
-      <c r="F94" s="39" t="s">
+      <c r="F96" s="39" t="s">
         <v>137</v>
       </c>
-      <c r="G94" s="15"/>
-      <c r="H94" s="18"/>
-      <c r="I94" s="33"/>
-    </row>
-    <row r="95" spans="1:26" s="61" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A95" s="34"/>
-      <c r="B95" s="35"/>
-      <c r="C95" s="35"/>
-      <c r="D95" s="35"/>
-      <c r="E95" s="36">
-        <f>SUM(E78:E94)</f>
+      <c r="G96" s="15"/>
+      <c r="H96" s="18"/>
+      <c r="I96" s="33"/>
+    </row>
+    <row r="97" spans="1:26" s="61" customFormat="1" ht="19.5" customHeight="1">
+      <c r="A97" s="34"/>
+      <c r="B97" s="35"/>
+      <c r="C97" s="35"/>
+      <c r="D97" s="35"/>
+      <c r="E97" s="36">
+        <f>SUM(E80:E96)</f>
         <v>349.20000000000005</v>
       </c>
-      <c r="F95" s="55"/>
-      <c r="G95" s="35"/>
-      <c r="H95" s="18" t="str">
-        <f>IF(F90&gt;0,LEFT(F90,20),"ZZZ")</f>
+      <c r="F97" s="55"/>
+      <c r="G97" s="35"/>
+      <c r="H97" s="18" t="str">
+        <f>IF(F92&gt;0,LEFT(F92,20),"ZZZ")</f>
         <v>https://www.servocit</v>
       </c>
-      <c r="I95" s="33"/>
-    </row>
-    <row r="96" spans="1:26" s="61" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A96" s="41" t="s">
+      <c r="I97" s="33"/>
+    </row>
+    <row r="98" spans="1:26" s="61" customFormat="1" ht="19.5" customHeight="1">
+      <c r="A98" s="41" t="s">
         <v>180</v>
       </c>
-      <c r="B96" s="28"/>
-      <c r="C96" s="28"/>
-      <c r="D96" s="28"/>
-      <c r="E96" s="28"/>
-      <c r="F96" s="56"/>
-      <c r="G96" s="28"/>
-      <c r="H96" s="28"/>
-      <c r="I96" s="28"/>
-    </row>
-    <row r="97" spans="1:26" s="61" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A97" s="34" t="s">
+      <c r="B98" s="28"/>
+      <c r="C98" s="28"/>
+      <c r="D98" s="28"/>
+      <c r="E98" s="28"/>
+      <c r="F98" s="56"/>
+      <c r="G98" s="28"/>
+      <c r="H98" s="28"/>
+      <c r="I98" s="28"/>
+    </row>
+    <row r="99" spans="1:26" s="61" customFormat="1" ht="19.5" customHeight="1">
+      <c r="A99" s="34" t="s">
         <v>181</v>
       </c>
-      <c r="B97" s="35">
+      <c r="B99" s="35">
         <v>1</v>
       </c>
-      <c r="C97" s="35">
+      <c r="C99" s="35">
         <v>1</v>
       </c>
-      <c r="D97" s="36">
+      <c r="D99" s="36">
         <v>20</v>
       </c>
-      <c r="E97" s="36">
-        <f t="shared" ref="E97:E98" si="12">D97*C97</f>
+      <c r="E99" s="36">
+        <f t="shared" ref="E99:E100" si="12">D99*C99</f>
         <v>20</v>
       </c>
-      <c r="F97" s="59" t="s">
+      <c r="F99" s="59" t="s">
         <v>183</v>
       </c>
-      <c r="G97" s="35"/>
-      <c r="H97" s="35"/>
-      <c r="I97" s="35"/>
-    </row>
-    <row r="98" spans="1:26" s="61" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A98" s="34" t="s">
+      <c r="G99" s="35"/>
+      <c r="H99" s="35"/>
+      <c r="I99" s="35"/>
+    </row>
+    <row r="100" spans="1:26" s="61" customFormat="1" ht="19.5" customHeight="1">
+      <c r="A100" s="34" t="s">
         <v>182</v>
       </c>
-      <c r="B98" s="35">
+      <c r="B100" s="35">
         <v>1</v>
       </c>
-      <c r="C98" s="35">
+      <c r="C100" s="35">
         <v>1</v>
       </c>
-      <c r="D98" s="43">
+      <c r="D100" s="43">
         <v>1.5</v>
       </c>
-      <c r="E98" s="36">
+      <c r="E100" s="36">
         <f t="shared" si="12"/>
         <v>1.5</v>
       </c>
-      <c r="F98" s="59" t="s">
+      <c r="F100" s="59" t="s">
         <v>184</v>
       </c>
-      <c r="G98" s="35"/>
-      <c r="H98" s="35"/>
-      <c r="I98" s="35"/>
-    </row>
-    <row r="99" spans="1:26" ht="19.5" customHeight="1">
-      <c r="A99" s="34"/>
-      <c r="B99" s="35"/>
-      <c r="C99" s="35"/>
-      <c r="D99" s="35"/>
-      <c r="E99" s="36">
-        <f>SUM((E97:E98))</f>
+      <c r="G100" s="35"/>
+      <c r="H100" s="35"/>
+      <c r="I100" s="35"/>
+    </row>
+    <row r="101" spans="1:26" ht="19.5" customHeight="1">
+      <c r="A101" s="34"/>
+      <c r="B101" s="35"/>
+      <c r="C101" s="35"/>
+      <c r="D101" s="35"/>
+      <c r="E101" s="36">
+        <f>SUM((E99:E100))</f>
         <v>21.5</v>
       </c>
-      <c r="F99" s="55"/>
-      <c r="G99" s="35"/>
-      <c r="H99" s="18" t="str">
-        <f>IF(F94&gt;0,LEFT(F94,20),"ZZZ")</f>
+      <c r="F101" s="55"/>
+      <c r="G101" s="35"/>
+      <c r="H101" s="18" t="str">
+        <f>IF(F96&gt;0,LEFT(F96,20),"ZZZ")</f>
         <v>https://www.servocit</v>
       </c>
-      <c r="I99" s="15"/>
-      <c r="J99" s="1"/>
-      <c r="K99" s="1"/>
-      <c r="L99" s="1"/>
-      <c r="M99" s="1"/>
-      <c r="N99" s="1"/>
-      <c r="O99" s="1"/>
-      <c r="P99" s="1"/>
-      <c r="Q99" s="1"/>
-      <c r="R99" s="1"/>
-      <c r="S99" s="1"/>
-      <c r="T99" s="1"/>
-      <c r="U99" s="1"/>
-      <c r="V99" s="1"/>
-      <c r="W99" s="1"/>
-      <c r="X99" s="1"/>
-      <c r="Y99" s="1"/>
-      <c r="Z99" s="1"/>
-    </row>
-    <row r="100" spans="1:26" s="47" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A100" s="41" t="s">
+      <c r="I101" s="15"/>
+      <c r="J101" s="1"/>
+      <c r="K101" s="1"/>
+      <c r="L101" s="1"/>
+      <c r="M101" s="1"/>
+      <c r="N101" s="1"/>
+      <c r="O101" s="1"/>
+      <c r="P101" s="1"/>
+      <c r="Q101" s="1"/>
+      <c r="R101" s="1"/>
+      <c r="S101" s="1"/>
+      <c r="T101" s="1"/>
+      <c r="U101" s="1"/>
+      <c r="V101" s="1"/>
+      <c r="W101" s="1"/>
+      <c r="X101" s="1"/>
+      <c r="Y101" s="1"/>
+      <c r="Z101" s="1"/>
+    </row>
+    <row r="102" spans="1:26" s="47" customFormat="1" ht="19.5" customHeight="1">
+      <c r="A102" s="41" t="s">
         <v>143</v>
       </c>
-      <c r="B100" s="28"/>
-      <c r="C100" s="28"/>
-      <c r="D100" s="28"/>
-      <c r="E100" s="28"/>
-      <c r="F100" s="56"/>
-      <c r="G100" s="28"/>
-      <c r="H100" s="28"/>
-      <c r="I100" s="28"/>
-    </row>
-    <row r="101" spans="1:26" s="47" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A101" s="34" t="s">
-        <v>144</v>
-      </c>
-      <c r="B101" s="35">
-        <v>3</v>
-      </c>
-      <c r="C101" s="35">
-        <v>1</v>
-      </c>
-      <c r="D101" s="36">
-        <v>1.5</v>
-      </c>
-      <c r="E101" s="36">
-        <f t="shared" ref="E101:E104" si="13">D101*C101</f>
-        <v>1.5</v>
-      </c>
-      <c r="F101" s="59" t="s">
-        <v>142</v>
-      </c>
-      <c r="G101" s="35"/>
-      <c r="H101" s="35"/>
-      <c r="I101" s="35"/>
-    </row>
-    <row r="102" spans="1:26" s="47" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A102" s="34" t="s">
-        <v>161</v>
-      </c>
-      <c r="B102" s="35">
-        <v>1</v>
-      </c>
-      <c r="C102" s="35">
-        <v>1</v>
-      </c>
-      <c r="D102" s="43">
-        <v>11.95</v>
-      </c>
-      <c r="E102" s="36">
-        <f t="shared" si="13"/>
-        <v>11.95</v>
-      </c>
-      <c r="F102" s="39" t="s">
-        <v>160</v>
-      </c>
-      <c r="G102" s="35"/>
-      <c r="H102" s="35"/>
-      <c r="I102" s="35"/>
+      <c r="B102" s="28"/>
+      <c r="C102" s="28"/>
+      <c r="D102" s="28"/>
+      <c r="E102" s="28"/>
+      <c r="F102" s="56"/>
+      <c r="G102" s="28"/>
+      <c r="H102" s="28"/>
+      <c r="I102" s="28"/>
     </row>
     <row r="103" spans="1:26" s="47" customFormat="1" ht="19.5" customHeight="1">
       <c r="A103" s="34" t="s">
-        <v>162</v>
+        <v>144</v>
       </c>
       <c r="B103" s="35">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C103" s="35">
         <v>1</v>
       </c>
-      <c r="D103" s="43">
-        <v>11.95</v>
+      <c r="D103" s="36">
+        <v>1.5</v>
       </c>
       <c r="E103" s="36">
-        <f t="shared" si="13"/>
-        <v>11.95</v>
-      </c>
-      <c r="F103" s="39" t="s">
-        <v>163</v>
+        <f t="shared" ref="E103:E106" si="13">D103*C103</f>
+        <v>1.5</v>
+      </c>
+      <c r="F103" s="59" t="s">
+        <v>142</v>
       </c>
       <c r="G103" s="35"/>
       <c r="H103" s="35"/>
@@ -5792,7 +5807,7 @@
     </row>
     <row r="104" spans="1:26" s="47" customFormat="1" ht="19.5" customHeight="1">
       <c r="A104" s="34" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="B104" s="35">
         <v>1</v>
@@ -5808,7 +5823,7 @@
         <v>11.95</v>
       </c>
       <c r="F104" s="39" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="G104" s="35"/>
       <c r="H104" s="35"/>
@@ -5816,7 +5831,7 @@
     </row>
     <row r="105" spans="1:26" s="47" customFormat="1" ht="19.5" customHeight="1">
       <c r="A105" s="34" t="s">
-        <v>146</v>
+        <v>162</v>
       </c>
       <c r="B105" s="35">
         <v>1</v>
@@ -5824,15 +5839,15 @@
       <c r="C105" s="35">
         <v>1</v>
       </c>
-      <c r="D105" s="35">
-        <v>0.69</v>
+      <c r="D105" s="43">
+        <v>11.95</v>
       </c>
       <c r="E105" s="36">
-        <f t="shared" ref="E105:E107" si="14">D105*C105</f>
-        <v>0.69</v>
-      </c>
-      <c r="F105" s="55" t="s">
-        <v>145</v>
+        <f t="shared" si="13"/>
+        <v>11.95</v>
+      </c>
+      <c r="F105" s="39" t="s">
+        <v>163</v>
       </c>
       <c r="G105" s="35"/>
       <c r="H105" s="35"/>
@@ -5840,23 +5855,23 @@
     </row>
     <row r="106" spans="1:26" s="47" customFormat="1" ht="19.5" customHeight="1">
       <c r="A106" s="34" t="s">
-        <v>148</v>
+        <v>165</v>
       </c>
       <c r="B106" s="35">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C106" s="35">
-        <v>2</v>
-      </c>
-      <c r="D106" s="35">
-        <v>0.44</v>
+        <v>1</v>
+      </c>
+      <c r="D106" s="43">
+        <v>11.95</v>
       </c>
       <c r="E106" s="36">
-        <f t="shared" ref="E106" si="15">D106*C106</f>
-        <v>0.88</v>
-      </c>
-      <c r="F106" s="55" t="s">
-        <v>147</v>
+        <f t="shared" si="13"/>
+        <v>11.95</v>
+      </c>
+      <c r="F106" s="39" t="s">
+        <v>164</v>
       </c>
       <c r="G106" s="35"/>
       <c r="H106" s="35"/>
@@ -5864,107 +5879,101 @@
     </row>
     <row r="107" spans="1:26" s="47" customFormat="1" ht="19.5" customHeight="1">
       <c r="A107" s="34" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B107" s="35">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C107" s="35">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D107" s="35">
-        <v>0.44</v>
+        <v>0.69</v>
       </c>
       <c r="E107" s="36">
-        <f t="shared" si="14"/>
-        <v>0.88</v>
+        <f t="shared" ref="E107:E109" si="14">D107*C107</f>
+        <v>0.69</v>
       </c>
       <c r="F107" s="55" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="G107" s="35"/>
       <c r="H107" s="35"/>
       <c r="I107" s="35"/>
     </row>
-    <row r="108" spans="1:26" s="48" customFormat="1" ht="19.5" customHeight="1" thickBot="1">
-      <c r="A108" s="34"/>
-      <c r="B108" s="35"/>
-      <c r="C108" s="50"/>
-      <c r="D108" s="50"/>
-      <c r="E108" s="62">
-        <f>SUM(E101:E107)</f>
-        <v>39.799999999999997</v>
-      </c>
-      <c r="F108" s="55"/>
+    <row r="108" spans="1:26" s="47" customFormat="1" ht="19.5" customHeight="1">
+      <c r="A108" s="34" t="s">
+        <v>148</v>
+      </c>
+      <c r="B108" s="35">
+        <v>2</v>
+      </c>
+      <c r="C108" s="35">
+        <v>2</v>
+      </c>
+      <c r="D108" s="35">
+        <v>0.44</v>
+      </c>
+      <c r="E108" s="36">
+        <f t="shared" ref="E108" si="15">D108*C108</f>
+        <v>0.88</v>
+      </c>
+      <c r="F108" s="55" t="s">
+        <v>147</v>
+      </c>
       <c r="G108" s="35"/>
       <c r="H108" s="35"/>
       <c r="I108" s="35"/>
     </row>
-    <row r="109" spans="1:26" ht="19.5" customHeight="1" thickBot="1">
-      <c r="A109" s="47"/>
-      <c r="B109" s="1"/>
-      <c r="C109" s="53"/>
-      <c r="D109" s="52" t="s">
+    <row r="109" spans="1:26" s="47" customFormat="1" ht="19.5" customHeight="1">
+      <c r="A109" s="34" t="s">
+        <v>148</v>
+      </c>
+      <c r="B109" s="35">
+        <v>2</v>
+      </c>
+      <c r="C109" s="35">
+        <v>2</v>
+      </c>
+      <c r="D109" s="35">
+        <v>0.44</v>
+      </c>
+      <c r="E109" s="36">
+        <f t="shared" si="14"/>
+        <v>0.88</v>
+      </c>
+      <c r="F109" s="55" t="s">
+        <v>147</v>
+      </c>
+      <c r="G109" s="35"/>
+      <c r="H109" s="35"/>
+      <c r="I109" s="35"/>
+    </row>
+    <row r="110" spans="1:26" s="48" customFormat="1" ht="19.5" customHeight="1" thickBot="1">
+      <c r="A110" s="34"/>
+      <c r="B110" s="35"/>
+      <c r="C110" s="50"/>
+      <c r="D110" s="50"/>
+      <c r="E110" s="62">
+        <f>SUM(E103:E109)</f>
+        <v>39.799999999999997</v>
+      </c>
+      <c r="F110" s="55"/>
+      <c r="G110" s="35"/>
+      <c r="H110" s="35"/>
+      <c r="I110" s="35"/>
+    </row>
+    <row r="111" spans="1:26" ht="19.5" customHeight="1" thickBot="1">
+      <c r="A111" s="47"/>
+      <c r="B111" s="1"/>
+      <c r="C111" s="53"/>
+      <c r="D111" s="52" t="s">
         <v>172</v>
       </c>
-      <c r="E109" s="51">
-        <f>SUM(E108,E99,E95,E76,E46,E40,E14)</f>
-        <v>1224.6500000000001</v>
-      </c>
-      <c r="G109" s="1"/>
-      <c r="H109" s="1"/>
-      <c r="I109" s="1"/>
-      <c r="J109" s="1"/>
-      <c r="K109" s="1"/>
-      <c r="L109" s="1"/>
-      <c r="M109" s="1"/>
-      <c r="N109" s="1"/>
-      <c r="O109" s="1"/>
-      <c r="P109" s="1"/>
-      <c r="Q109" s="1"/>
-      <c r="R109" s="1"/>
-      <c r="S109" s="1"/>
-      <c r="T109" s="1"/>
-      <c r="U109" s="1"/>
-      <c r="V109" s="1"/>
-      <c r="W109" s="1"/>
-      <c r="X109" s="1"/>
-      <c r="Y109" s="1"/>
-      <c r="Z109" s="1"/>
-    </row>
-    <row r="110" spans="1:26" ht="19.5" customHeight="1">
-      <c r="A110" s="1"/>
-      <c r="B110" s="1"/>
-      <c r="C110" s="1"/>
-      <c r="D110" s="1"/>
-      <c r="E110" s="1"/>
-      <c r="G110" s="1"/>
-      <c r="H110" s="1"/>
-      <c r="I110" s="1"/>
-      <c r="J110" s="1"/>
-      <c r="K110" s="1"/>
-      <c r="L110" s="1"/>
-      <c r="M110" s="1"/>
-      <c r="N110" s="1"/>
-      <c r="O110" s="1"/>
-      <c r="P110" s="1"/>
-      <c r="Q110" s="1"/>
-      <c r="R110" s="1"/>
-      <c r="S110" s="1"/>
-      <c r="T110" s="1"/>
-      <c r="U110" s="1"/>
-      <c r="V110" s="1"/>
-      <c r="W110" s="1"/>
-      <c r="X110" s="1"/>
-      <c r="Y110" s="1"/>
-      <c r="Z110" s="1"/>
-    </row>
-    <row r="111" spans="1:26" ht="19.5" customHeight="1">
-      <c r="A111" s="1"/>
-      <c r="B111" s="1"/>
-      <c r="C111" s="1"/>
-      <c r="D111" s="1"/>
-      <c r="E111" s="1"/>
+      <c r="E111" s="51">
+        <f>SUM(E110,E101,E97,E78,E46,E40,E14)</f>
+        <v>1241.9900000000002</v>
+      </c>
       <c r="G111" s="1"/>
       <c r="H111" s="1"/>
       <c r="I111" s="1"/>
@@ -29341,20 +29350,68 @@
       <c r="Y976" s="1"/>
       <c r="Z976" s="1"/>
     </row>
+    <row r="977" spans="1:26" ht="19.5" customHeight="1">
+      <c r="A977" s="1"/>
+      <c r="B977" s="1"/>
+      <c r="C977" s="1"/>
+      <c r="D977" s="1"/>
+      <c r="E977" s="1"/>
+      <c r="G977" s="1"/>
+      <c r="H977" s="1"/>
+      <c r="I977" s="1"/>
+      <c r="J977" s="1"/>
+      <c r="K977" s="1"/>
+      <c r="L977" s="1"/>
+      <c r="M977" s="1"/>
+      <c r="N977" s="1"/>
+      <c r="O977" s="1"/>
+      <c r="P977" s="1"/>
+      <c r="Q977" s="1"/>
+      <c r="R977" s="1"/>
+      <c r="S977" s="1"/>
+      <c r="T977" s="1"/>
+      <c r="U977" s="1"/>
+      <c r="V977" s="1"/>
+      <c r="W977" s="1"/>
+      <c r="X977" s="1"/>
+      <c r="Y977" s="1"/>
+      <c r="Z977" s="1"/>
+    </row>
+    <row r="978" spans="1:26" ht="19.5" customHeight="1">
+      <c r="A978" s="1"/>
+      <c r="B978" s="1"/>
+      <c r="C978" s="1"/>
+      <c r="D978" s="1"/>
+      <c r="E978" s="1"/>
+      <c r="G978" s="1"/>
+      <c r="H978" s="1"/>
+      <c r="I978" s="1"/>
+      <c r="J978" s="1"/>
+      <c r="K978" s="1"/>
+      <c r="L978" s="1"/>
+      <c r="M978" s="1"/>
+      <c r="N978" s="1"/>
+      <c r="O978" s="1"/>
+      <c r="P978" s="1"/>
+      <c r="Q978" s="1"/>
+      <c r="R978" s="1"/>
+      <c r="S978" s="1"/>
+      <c r="T978" s="1"/>
+      <c r="U978" s="1"/>
+      <c r="V978" s="1"/>
+      <c r="W978" s="1"/>
+      <c r="X978" s="1"/>
+      <c r="Y978" s="1"/>
+      <c r="Z978" s="1"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A2:Z99" xr:uid="{00000000-0009-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Z99">
-      <sortCondition ref="H2:H99"/>
-      <sortCondition ref="A2:A99"/>
+  <autoFilter ref="A2:Z101" xr:uid="{00000000-0009-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Z101">
+      <sortCondition ref="H2:H101"/>
+      <sortCondition ref="A2:A101"/>
     </sortState>
   </autoFilter>
   <mergeCells count="18">
-    <mergeCell ref="F88:G88"/>
-    <mergeCell ref="F48:G48"/>
-    <mergeCell ref="F49:G49"/>
-    <mergeCell ref="F50:G50"/>
-    <mergeCell ref="F51:G51"/>
-    <mergeCell ref="F52:G52"/>
     <mergeCell ref="A1:I1"/>
     <mergeCell ref="F43:G43"/>
     <mergeCell ref="F45:G45"/>
@@ -29367,6 +29424,12 @@
     <mergeCell ref="F36:G36"/>
     <mergeCell ref="F37:G37"/>
     <mergeCell ref="F38:G38"/>
+    <mergeCell ref="F90:G90"/>
+    <mergeCell ref="F48:G48"/>
+    <mergeCell ref="F49:G49"/>
+    <mergeCell ref="F50:G50"/>
+    <mergeCell ref="F51:G51"/>
+    <mergeCell ref="F52:G52"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F4" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
@@ -29378,26 +29441,26 @@
     <hyperlink ref="F42" r:id="rId7" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
     <hyperlink ref="F45" r:id="rId8" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
     <hyperlink ref="F48" r:id="rId9" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
-    <hyperlink ref="F78" r:id="rId10" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
-    <hyperlink ref="F79" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
-    <hyperlink ref="F80" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
-    <hyperlink ref="F81" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
-    <hyperlink ref="F82" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00003E000000}"/>
-    <hyperlink ref="F83" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
-    <hyperlink ref="F84" r:id="rId16" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
-    <hyperlink ref="F85" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
-    <hyperlink ref="F86" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000042000000}"/>
-    <hyperlink ref="F87" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000043000000}"/>
-    <hyperlink ref="F89" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000044000000}"/>
-    <hyperlink ref="F90" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000045000000}"/>
-    <hyperlink ref="F91" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000046000000}"/>
-    <hyperlink ref="F92" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000047000000}"/>
-    <hyperlink ref="F93" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000048000000}"/>
-    <hyperlink ref="F94" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000049000000}"/>
+    <hyperlink ref="F80" r:id="rId10" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
+    <hyperlink ref="F81" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
+    <hyperlink ref="F82" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
+    <hyperlink ref="F83" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
+    <hyperlink ref="F84" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00003E000000}"/>
+    <hyperlink ref="F85" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
+    <hyperlink ref="F86" r:id="rId16" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
+    <hyperlink ref="F87" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
+    <hyperlink ref="F88" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000042000000}"/>
+    <hyperlink ref="F89" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000043000000}"/>
+    <hyperlink ref="F91" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000044000000}"/>
+    <hyperlink ref="F92" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000045000000}"/>
+    <hyperlink ref="F93" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000046000000}"/>
+    <hyperlink ref="F94" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000047000000}"/>
+    <hyperlink ref="F95" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000048000000}"/>
+    <hyperlink ref="F96" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000049000000}"/>
     <hyperlink ref="F35" r:id="rId26" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
     <hyperlink ref="F43" r:id="rId27" xr:uid="{454FB29B-EB5B-45E2-9934-2869B74B5DF9}"/>
-    <hyperlink ref="F75" r:id="rId28" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
-    <hyperlink ref="F74" r:id="rId29" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
+    <hyperlink ref="F76" r:id="rId28" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
+    <hyperlink ref="F75" r:id="rId29" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
     <hyperlink ref="F73" r:id="rId30" xr:uid="{00000000-0004-0000-0000-000037000000}"/>
     <hyperlink ref="F72" r:id="rId31" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
     <hyperlink ref="F71" r:id="rId32" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
@@ -29442,15 +29505,16 @@
     <hyperlink ref="F9" r:id="rId71" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
     <hyperlink ref="F17" r:id="rId72" xr:uid="{AE212094-AA82-4C0C-AF1E-4B51D8F797FA}"/>
     <hyperlink ref="F18" r:id="rId73" xr:uid="{11BE5682-BF9B-4375-8CE6-F3E0F91E703D}"/>
-    <hyperlink ref="F88" r:id="rId74" xr:uid="{925FCD95-4665-4481-98DD-84FCC604B9F9}"/>
-    <hyperlink ref="F97" r:id="rId75" xr:uid="{F4B34013-2538-47A6-AA92-2B4AD39FF242}"/>
-    <hyperlink ref="F98" r:id="rId76" xr:uid="{6A01326A-3ECC-488B-A6D3-9309B5EBA0BE}"/>
+    <hyperlink ref="F90" r:id="rId74" xr:uid="{925FCD95-4665-4481-98DD-84FCC604B9F9}"/>
+    <hyperlink ref="F99" r:id="rId75" xr:uid="{F4B34013-2538-47A6-AA92-2B4AD39FF242}"/>
+    <hyperlink ref="F100" r:id="rId76" xr:uid="{6A01326A-3ECC-488B-A6D3-9309B5EBA0BE}"/>
     <hyperlink ref="F37" r:id="rId77" xr:uid="{A09FCC8C-EED4-4230-809F-AB1E9B36A50C}"/>
-    <hyperlink ref="F101" r:id="rId78" xr:uid="{240D3D57-31EF-4068-B699-D4755C52F2ED}"/>
+    <hyperlink ref="F103" r:id="rId78" xr:uid="{240D3D57-31EF-4068-B699-D4755C52F2ED}"/>
     <hyperlink ref="F36" r:id="rId79" xr:uid="{3A737759-F3C2-43EC-A0BD-11C12A560D0A}"/>
+    <hyperlink ref="F74" r:id="rId80" xr:uid="{CEA8D239-A039-4B44-8A3D-32C3480AE38F}"/>
   </hyperlinks>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup scale="72" orientation="portrait" r:id="rId80"/>
+  <pageSetup scale="72" orientation="portrait" r:id="rId81"/>
   <headerFooter>
     <oddFooter>&amp;C000000&amp;P</oddFooter>
   </headerFooter>

</xml_diff>